<commit_message>
Update Admin Task List & Summary.xlsx
</commit_message>
<xml_diff>
--- a/docs/Admin Task List & Summary.xlsx
+++ b/docs/Admin Task List & Summary.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="92">
   <si>
     <t xml:space="preserve">Sr. NO </t>
   </si>
@@ -400,9 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
@@ -411,11 +408,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
+  <dxfs count="74">
     <dxf>
       <font>
         <name val="Eras Medium ITC"/>
@@ -531,66 +531,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <name val="Eras Medium ITC"/>
         <scheme val="none"/>
       </font>
@@ -701,369 +641,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Eras Medium ITC"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1334,7 +911,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="shaheryar" refreshedDate="45584.527410879629" createdVersion="8" refreshedVersion="5" minRefreshableVersion="3" recordCount="141">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="shaheryar" refreshedDate="45586.538322453707" createdVersion="8" refreshedVersion="5" minRefreshableVersion="3" recordCount="140">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
@@ -1352,10 +929,10 @@
         <s v="Investigation"/>
         <s v="Main"/>
         <s v="Medicine"/>
+        <s v="LookUps"/>
         <s v="Support Tickets"/>
         <s v="Deit Facts"/>
         <s v="System"/>
-        <s v="LookUps"/>
         <s v="ClinTa Web-Builder"/>
         <s v="ClinTa Health Care"/>
         <s v="ClinTa Extended"/>
@@ -1388,7 +965,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="141">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="140">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -1451,7 +1028,7 @@
     <s v="Diseases"/>
     <s v="Listing"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="9"/>
@@ -1459,7 +1036,7 @@
     <s v="Diseases"/>
     <s v="Add"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="10"/>
@@ -1467,7 +1044,7 @@
     <s v="Diseases"/>
     <s v="Delete"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="11"/>
@@ -1475,7 +1052,7 @@
     <s v="Diseases"/>
     <s v="Update"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="12"/>
@@ -2015,43 +1592,43 @@
   </r>
   <r>
     <n v="79"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="LookUps (Nav)"/>
     <s v="Listing"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="80"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="LookUps (Nav)"/>
     <s v="Add"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="81"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="LookUps (Nav)"/>
     <s v="Update"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="82"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="LookUps (Nav)"/>
     <s v="Delete"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="83"/>
-    <x v="6"/>
+    <x v="8"/>
     <s v="LookUps (Nav)"/>
     <s v="Filters"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="84"/>
@@ -2111,7 +1688,7 @@
   </r>
   <r>
     <n v="91"/>
-    <x v="8"/>
+    <x v="9"/>
     <s v="ClinTa Extended"/>
     <s v="Filter"/>
     <m/>
@@ -2119,7 +1696,7 @@
   </r>
   <r>
     <n v="92"/>
-    <x v="8"/>
+    <x v="9"/>
     <s v="ClinTa Extended"/>
     <s v="Crud"/>
     <m/>
@@ -2127,7 +1704,7 @@
   </r>
   <r>
     <n v="93"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Fruits"/>
     <s v="Crud"/>
     <m/>
@@ -2135,7 +1712,7 @@
   </r>
   <r>
     <n v="94"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Vegetable"/>
     <s v="Crud"/>
     <m/>
@@ -2143,7 +1720,7 @@
   </r>
   <r>
     <n v="95"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Pulses-Grains"/>
     <s v="Crud"/>
     <m/>
@@ -2151,7 +1728,7 @@
   </r>
   <r>
     <n v="96"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Dry Fruits"/>
     <s v="Crud"/>
     <m/>
@@ -2159,7 +1736,7 @@
   </r>
   <r>
     <n v="97"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Miscellaneous"/>
     <s v="Crud"/>
     <m/>
@@ -2167,23 +1744,15 @@
   </r>
   <r>
     <n v="98"/>
-    <x v="10"/>
+    <x v="11"/>
     <s v=" Users"/>
     <s v="Add"/>
     <m/>
     <x v="1"/>
   </r>
   <r>
-    <n v="99"/>
-    <x v="11"/>
-    <s v="List"/>
-    <s v="Crud"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="100"/>
-    <x v="11"/>
+    <x v="8"/>
     <s v="List"/>
     <s v="Filter"/>
     <m/>
@@ -2191,15 +1760,15 @@
   </r>
   <r>
     <n v="101"/>
-    <x v="11"/>
+    <x v="8"/>
     <s v="LookUps Options"/>
     <s v="Crud"/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="102"/>
-    <x v="11"/>
+    <x v="8"/>
     <s v="LookUps Options"/>
     <s v="Filter"/>
     <m/>
@@ -2471,7 +2040,7 @@
   </r>
   <r>
     <n v="135"/>
-    <x v="10"/>
+    <x v="11"/>
     <s v=" Users"/>
     <s v="Update"/>
     <m/>
@@ -2479,7 +2048,7 @@
   </r>
   <r>
     <n v="136"/>
-    <x v="10"/>
+    <x v="11"/>
     <s v=" Users"/>
     <s v="Delete"/>
     <m/>
@@ -2487,7 +2056,7 @@
   </r>
   <r>
     <n v="137"/>
-    <x v="10"/>
+    <x v="11"/>
     <s v=" Users"/>
     <s v="Listing"/>
     <m/>
@@ -2521,7 +2090,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Product Segments" colHeaderCaption=" ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Product Segments" colHeaderCaption=" ">
   <location ref="A3:D21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -2533,16 +2102,16 @@
         <item x="15"/>
         <item x="12"/>
         <item x="1"/>
-        <item x="9"/>
+        <item x="10"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
-        <item x="11"/>
+        <item x="8"/>
         <item x="6"/>
         <item x="7"/>
-        <item x="8"/>
-        <item x="10"/>
+        <item x="9"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2632,83 +2201,83 @@
     <dataField name=" " fld="5" subtotal="count" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="21">
-    <format dxfId="125">
+    <format dxfId="73">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="72">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="123">
+    <format dxfId="71">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="70">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="69">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="68">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="118">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="116">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="63">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="114">
+    <format dxfId="62">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="113">
+    <format dxfId="61">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="60">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="111">
+    <format dxfId="59">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="110">
+    <format dxfId="58">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="109">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="107">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="105">
+    <format dxfId="53">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2725,18 +2294,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F142" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
-  <autoFilter ref="A1:F142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F141" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:F141">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LookUps"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:F131">
     <sortCondition ref="A4:A131"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Sr. NO " dataDxfId="102"/>
-    <tableColumn id="1" name="Product" dataDxfId="101"/>
-    <tableColumn id="3" name="Segment" dataDxfId="100"/>
-    <tableColumn id="6" name="Sub Segment" dataDxfId="99"/>
-    <tableColumn id="4" name="Task" dataDxfId="98"/>
-    <tableColumn id="5" name="Status" dataDxfId="97"/>
+    <tableColumn id="2" name="Sr. NO " dataDxfId="50"/>
+    <tableColumn id="1" name="Product" dataDxfId="49"/>
+    <tableColumn id="3" name="Segment" dataDxfId="48"/>
+    <tableColumn id="6" name="Sub Segment" dataDxfId="47"/>
+    <tableColumn id="4" name="Task" dataDxfId="46"/>
+    <tableColumn id="5" name="Status" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3063,7 +2638,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3076,246 +2651,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="4.5" customHeight="1"/>
     <row r="3" spans="1:4" ht="18.75" hidden="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10">
-        <v>9</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="B6" s="9">
+        <v>9</v>
+      </c>
+      <c r="C6" s="9">
         <v>7</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9">
         <v>6</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
         <v>2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9">
         <v>8</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10">
+      <c r="B12" s="9">
         <v>4</v>
       </c>
-      <c r="D12" s="10">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
         <v>7</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>26</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>12</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9">
         <v>10</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10">
+      <c r="B16" s="9">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75">
+      <c r="A17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9">
+        <v>18</v>
+      </c>
+      <c r="D17" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75">
+      <c r="A18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75">
+      <c r="A19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75">
+      <c r="A20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="9">
         <v>4</v>
       </c>
-      <c r="D16" s="10">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.75">
-      <c r="A17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10">
-        <v>23</v>
-      </c>
-      <c r="D17" s="10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75">
-      <c r="A18" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10">
-        <v>7</v>
-      </c>
-      <c r="D18" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75">
-      <c r="A19" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10">
-        <v>2</v>
-      </c>
-      <c r="D19" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75">
-      <c r="A20" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="10">
-        <v>4</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10">
-        <v>4</v>
-      </c>
-    </row>
     <row r="21" spans="1:4" ht="18.75">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="10">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10">
-        <v>97</v>
-      </c>
-      <c r="D21" s="10">
-        <v>141</v>
+      <c r="B21" s="9">
+        <v>54</v>
+      </c>
+      <c r="C21" s="9">
+        <v>86</v>
+      </c>
+      <c r="D21" s="9">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3328,11 +2905,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
+      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3365,14 +2942,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" ht="15.75" hidden="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3383,14 +2960,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75">
+    <row r="3" spans="1:6" ht="15.75" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3401,14 +2978,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6" ht="15.75" hidden="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3419,14 +2996,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75">
+    <row r="5" spans="1:6" ht="15.75" hidden="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3437,14 +3014,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75">
+    <row r="6" spans="1:6" ht="15.75" hidden="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -3455,14 +3032,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
+    <row r="7" spans="1:6" ht="15.75" hidden="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3473,14 +3050,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6" ht="15.75" hidden="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="1"/>
@@ -3489,14 +3066,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
+    <row r="9" spans="1:6" ht="15.75" hidden="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -3504,17 +3081,17 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" hidden="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -3522,17 +3099,17 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" hidden="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -3540,17 +3117,17 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" hidden="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -3558,17 +3135,17 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" hidden="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -3579,14 +3156,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75">
+    <row r="14" spans="1:6" ht="15.75" hidden="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -3597,14 +3174,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75">
+    <row r="15" spans="1:6" ht="15.75" hidden="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -3615,14 +3192,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75">
+    <row r="16" spans="1:6" ht="15.75" hidden="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -3633,14 +3210,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75">
+    <row r="17" spans="1:6" ht="15.75" hidden="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -3651,14 +3228,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75">
+    <row r="18" spans="1:6" ht="15.75" hidden="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3669,14 +3246,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75">
+    <row r="19" spans="1:6" ht="15.75" hidden="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -3687,14 +3264,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75">
+    <row r="20" spans="1:6" ht="15.75" hidden="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -3705,14 +3282,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75">
+    <row r="21" spans="1:6" ht="15.75" hidden="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -3723,14 +3300,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75">
+    <row r="22" spans="1:6" ht="15.75" hidden="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3741,14 +3318,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75">
+    <row r="23" spans="1:6" ht="15.75" hidden="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -3759,14 +3336,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75">
+    <row r="24" spans="1:6" ht="15.75" hidden="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -3777,14 +3354,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75">
+    <row r="25" spans="1:6" ht="15.75" hidden="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -3795,14 +3372,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6" ht="15.75" hidden="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3813,14 +3390,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75">
+    <row r="27" spans="1:6" ht="15.75" hidden="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3831,14 +3408,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75">
+    <row r="28" spans="1:6" ht="15.75" hidden="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -3849,14 +3426,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75">
+    <row r="29" spans="1:6" ht="15.75" hidden="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -3867,14 +3444,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75">
+    <row r="30" spans="1:6" ht="15.75" hidden="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -3885,14 +3462,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75">
+    <row r="31" spans="1:6" ht="15.75" hidden="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -3903,14 +3480,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75">
+    <row r="32" spans="1:6" ht="15.75" hidden="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -3921,14 +3498,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75">
+    <row r="33" spans="1:6" ht="15.75" hidden="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3939,14 +3516,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15.75" hidden="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -3957,14 +3534,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75">
+    <row r="35" spans="1:6" ht="15.75" hidden="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -3975,14 +3552,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75">
+    <row r="36" spans="1:6" ht="15.75" hidden="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -3993,14 +3570,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75">
+    <row r="37" spans="1:6" ht="15.75" hidden="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -4011,14 +3588,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75">
+    <row r="38" spans="1:6" ht="15.75" hidden="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4029,14 +3606,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75">
+    <row r="39" spans="1:6" ht="15.75" hidden="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -4047,14 +3624,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75">
+    <row r="40" spans="1:6" ht="15.75" hidden="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -4065,14 +3642,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75">
+    <row r="41" spans="1:6" ht="15.75" hidden="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -4083,14 +3660,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75">
+    <row r="42" spans="1:6" ht="15.75" hidden="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -4101,14 +3678,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75">
+    <row r="43" spans="1:6" ht="15.75" hidden="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -4119,14 +3696,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75">
+    <row r="44" spans="1:6" ht="15.75" hidden="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -4137,14 +3714,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75">
+    <row r="45" spans="1:6" ht="15.75" hidden="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -4155,14 +3732,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75">
+    <row r="46" spans="1:6" ht="15.75" hidden="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -4173,14 +3750,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75">
+    <row r="47" spans="1:6" ht="15.75" hidden="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -4191,14 +3768,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75">
+    <row r="48" spans="1:6" ht="15.75" hidden="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -4209,14 +3786,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75">
+    <row r="49" spans="1:6" ht="15.75" hidden="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -4227,14 +3804,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75">
+    <row r="50" spans="1:6" ht="15.75" hidden="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -4245,14 +3822,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75">
+    <row r="51" spans="1:6" ht="15.75" hidden="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -4263,14 +3840,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75">
+    <row r="52" spans="1:6" ht="15.75" hidden="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -4281,14 +3858,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75">
+    <row r="53" spans="1:6" ht="15.75" hidden="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -4299,14 +3876,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75">
+    <row r="54" spans="1:6" ht="15.75" hidden="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -4317,14 +3894,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75">
+    <row r="55" spans="1:6" ht="15.75" hidden="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -4335,14 +3912,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75">
+    <row r="56" spans="1:6" ht="15.75" hidden="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -4353,14 +3930,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75">
+    <row r="57" spans="1:6" ht="15.75" hidden="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -4371,14 +3948,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75">
+    <row r="58" spans="1:6" ht="15.75" hidden="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -4389,14 +3966,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75">
+    <row r="59" spans="1:6" ht="15.75" hidden="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -4407,14 +3984,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75">
+    <row r="60" spans="1:6" ht="15.75" hidden="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -4425,14 +4002,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75">
+    <row r="61" spans="1:6" ht="15.75" hidden="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -4443,14 +4020,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75">
+    <row r="62" spans="1:6" ht="15.75" hidden="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -4461,14 +4038,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75">
+    <row r="63" spans="1:6" ht="15.75" hidden="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -4479,14 +4056,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75">
+    <row r="64" spans="1:6" ht="15.75" hidden="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -4497,14 +4074,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75">
+    <row r="65" spans="1:6" ht="15.75" hidden="1">
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -4515,14 +4092,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75">
+    <row r="66" spans="1:6" ht="15.75" hidden="1">
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -4533,14 +4110,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75">
+    <row r="67" spans="1:6" ht="15.75" hidden="1">
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -4551,14 +4128,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75">
+    <row r="68" spans="1:6" ht="15.75" hidden="1">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -4569,14 +4146,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75">
+    <row r="69" spans="1:6" ht="15.75" hidden="1">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -4587,14 +4164,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75">
+    <row r="70" spans="1:6" ht="15.75" hidden="1">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -4605,14 +4182,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75">
+    <row r="71" spans="1:6" ht="15.75" hidden="1">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -4623,14 +4200,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75">
+    <row r="72" spans="1:6" ht="15.75" hidden="1">
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -4641,14 +4218,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75">
+    <row r="73" spans="1:6" ht="15.75" hidden="1">
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -4659,14 +4236,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75">
+    <row r="74" spans="1:6" ht="15.75" hidden="1">
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -4677,14 +4254,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75">
+    <row r="75" spans="1:6" ht="15.75" hidden="1">
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -4695,14 +4272,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75">
+    <row r="76" spans="1:6" ht="15.75" hidden="1">
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -4713,14 +4290,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75">
+    <row r="77" spans="1:6" ht="15.75" hidden="1">
       <c r="A77" s="1">
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -4731,14 +4308,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75">
+    <row r="78" spans="1:6" ht="15.75" hidden="1">
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -4749,14 +4326,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75">
+    <row r="79" spans="1:6" ht="15.75" hidden="1">
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -4771,10 +4348,10 @@
       <c r="A80" s="1">
         <v>79</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C80" s="5" t="s">
+      <c r="B80" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -4782,17 +4359,17 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75">
       <c r="A81" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C81" s="5" t="s">
+      <c r="B81" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -4800,17 +4377,17 @@
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75">
       <c r="A82" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C82" s="5" t="s">
+      <c r="B82" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -4818,17 +4395,17 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75">
       <c r="A83" s="1">
         <v>82</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C83" s="5" t="s">
+      <c r="B83" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -4836,17 +4413,17 @@
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75">
       <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C84" s="5" t="s">
+      <c r="B84" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -4854,17 +4431,17 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" hidden="1">
       <c r="A85" s="1">
         <v>84</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -4875,14 +4452,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.75">
+    <row r="86" spans="1:6" ht="15.75" hidden="1">
       <c r="A86" s="1">
         <v>85</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -4893,14 +4470,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.75">
+    <row r="87" spans="1:6" ht="15.75" hidden="1">
       <c r="A87" s="1">
         <v>86</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -4911,14 +4488,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75">
+    <row r="88" spans="1:6" ht="15.75" hidden="1">
       <c r="A88" s="1">
         <v>87</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -4929,14 +4506,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75">
+    <row r="89" spans="1:6" ht="15.75" hidden="1">
       <c r="A89" s="1">
         <v>88</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -4947,14 +4524,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.75">
+    <row r="90" spans="1:6" ht="15.75" hidden="1">
       <c r="A90" s="1">
         <v>89</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -4965,14 +4542,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.75">
+    <row r="91" spans="1:6" ht="15.75" hidden="1">
       <c r="A91" s="1">
         <v>90</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -4983,14 +4560,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.75">
+    <row r="92" spans="1:6" ht="15.75" hidden="1">
       <c r="A92" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -5001,14 +4578,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.75">
+    <row r="93" spans="1:6" ht="15.75" hidden="1">
       <c r="A93" s="1">
         <v>92</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -5019,14 +4596,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.75">
+    <row r="94" spans="1:6" ht="15.75" hidden="1">
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -5037,14 +4614,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.75">
+    <row r="95" spans="1:6" ht="15.75" hidden="1">
       <c r="A95" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -5055,14 +4632,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.75">
+    <row r="96" spans="1:6" ht="15.75" hidden="1">
       <c r="A96" s="1">
         <v>95</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -5073,14 +4650,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.75">
+    <row r="97" spans="1:6" ht="15.75" hidden="1">
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -5091,14 +4668,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.75">
+    <row r="98" spans="1:6" ht="15.75" hidden="1">
       <c r="A98" s="1">
         <v>97</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -5109,14 +4686,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.75">
+    <row r="99" spans="1:6" ht="15.75" hidden="1">
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="4" t="s">
         <v>85</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -5129,16 +4706,16 @@
     </row>
     <row r="100" spans="1:6" ht="15.75">
       <c r="A100" s="1">
-        <v>99</v>
-      </c>
-      <c r="B100" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
@@ -5147,69 +4724,69 @@
     </row>
     <row r="101" spans="1:6" ht="15.75">
       <c r="A101" s="1">
-        <v>100</v>
-      </c>
-      <c r="B101" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>8</v>
+      <c r="C101" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.75">
       <c r="A102" s="1">
-        <v>101</v>
-      </c>
-      <c r="B102" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.75">
+    <row r="103" spans="1:6" ht="15.75" hidden="1">
       <c r="A103" s="1">
-        <v>102</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.75">
+    <row r="104" spans="1:6" ht="15.75" hidden="1">
       <c r="A104" s="1">
-        <v>103</v>
-      </c>
-      <c r="B104" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D104" s="5" t="s">
+      <c r="C104" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="1"/>
@@ -5217,35 +4794,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.75">
+    <row r="105" spans="1:6" ht="15.75" hidden="1">
       <c r="A105" s="1">
-        <v>104</v>
-      </c>
-      <c r="B105" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>11</v>
+      <c r="C105" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.75">
+    <row r="106" spans="1:6" ht="15.75" hidden="1">
       <c r="A106" s="1">
-        <v>105</v>
-      </c>
-      <c r="B106" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D106" s="5" t="s">
+      <c r="C106" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D106" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E106" s="1"/>
@@ -5253,35 +4830,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.75">
+    <row r="107" spans="1:6" ht="15.75" hidden="1">
       <c r="A107" s="1">
-        <v>106</v>
-      </c>
-      <c r="B107" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>17</v>
+      <c r="C107" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.75">
+    <row r="108" spans="1:6" ht="15.75" hidden="1">
       <c r="A108" s="1">
-        <v>107</v>
-      </c>
-      <c r="B108" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D108" s="5" t="s">
+      <c r="C108" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="1"/>
@@ -5289,17 +4866,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.75">
+    <row r="109" spans="1:6" ht="15.75" hidden="1">
       <c r="A109" s="1">
-        <v>108</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D109" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E109" s="1"/>
@@ -5307,9 +4884,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.75">
+    <row r="110" spans="1:6" ht="15.75" hidden="1">
       <c r="A110" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>28</v>
@@ -5318,34 +4895,34 @@
         <v>29</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.75">
+    <row r="111" spans="1:6" ht="15.75" hidden="1">
       <c r="A111" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15.75">
+    <row r="112" spans="1:6" ht="15.75" hidden="1">
       <c r="A112" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>28</v>
@@ -5354,34 +4931,34 @@
         <v>30</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.75">
+    <row r="113" spans="1:6" ht="15.75" hidden="1">
       <c r="A113" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.75">
+    <row r="114" spans="1:6" ht="15.75" hidden="1">
       <c r="A114" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>28</v>
@@ -5390,40 +4967,40 @@
         <v>31</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.75">
+    <row r="115" spans="1:6" ht="15.75" hidden="1">
       <c r="A115" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.75">
+    <row r="116" spans="1:6" ht="15.75" hidden="1">
       <c r="A116" s="1">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -5433,15 +5010,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.75">
+    <row r="117" spans="1:6" ht="15.75" hidden="1">
       <c r="A117" s="1">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -5451,27 +5028,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.75">
+    <row r="118" spans="1:6" ht="15.75" hidden="1">
       <c r="A118" s="1">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.75">
+    <row r="119" spans="1:6" ht="15.75" hidden="1">
       <c r="A119" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>14</v>
@@ -5479,17 +5056,17 @@
       <c r="C119" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E119" s="1"/>
+      <c r="D119" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E119" s="2"/>
       <c r="F119" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.75">
+    <row r="120" spans="1:6" ht="15.75" hidden="1">
       <c r="A120" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>14</v>
@@ -5498,16 +5075,16 @@
         <v>16</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.75">
+    <row r="121" spans="1:6" ht="15.75" hidden="1">
       <c r="A121" s="1">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>14</v>
@@ -5516,14 +5093,14 @@
         <v>16</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" hidden="1">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -5534,16 +5111,16 @@
         <v>16</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="15.75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" hidden="1">
       <c r="A123" s="1">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>14</v>
@@ -5551,53 +5128,53 @@
       <c r="C123" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E123" s="2"/>
+      <c r="D123" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15.75">
+    <row r="124" spans="1:6" ht="15.75" hidden="1">
       <c r="A124" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15.75">
+    <row r="125" spans="1:6" ht="15.75" hidden="1">
       <c r="A125" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15.75" hidden="1">
       <c r="A126" s="1">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>14</v>
@@ -5605,17 +5182,17 @@
       <c r="C126" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E126" s="1"/>
+      <c r="D126" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E126" s="2"/>
       <c r="F126" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15.75">
+    <row r="127" spans="1:6" ht="15.75" hidden="1">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>14</v>
@@ -5624,16 +5201,16 @@
         <v>19</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15.75">
+    <row r="128" spans="1:6" ht="15.75" hidden="1">
       <c r="A128" s="1">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>14</v>
@@ -5642,112 +5219,112 @@
         <v>19</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15.75">
+    <row r="129" spans="1:6" ht="15.75" hidden="1">
       <c r="A129" s="1">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E129" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15.75">
+    <row r="130" spans="1:6" ht="15.75" hidden="1">
       <c r="A130" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" hidden="1">
       <c r="A131" s="1">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15.75">
+    <row r="132" spans="1:6" ht="15.75" hidden="1">
       <c r="A132" s="1">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15.75">
+    <row r="133" spans="1:6" ht="15.75" hidden="1">
       <c r="A133" s="1">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15.75">
+    <row r="134" spans="1:6" ht="15.75" hidden="1">
       <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>6</v>
+        <v>133</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>11</v>
@@ -5757,9 +5334,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15.75">
+    <row r="135" spans="1:6" ht="15.75" hidden="1">
       <c r="A135" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>26</v>
@@ -5768,88 +5345,88 @@
         <v>27</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15.75">
+    <row r="136" spans="1:6" ht="15.75" hidden="1">
       <c r="A136" s="1">
-        <v>134</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E136" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E136" s="2"/>
       <c r="F136" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15.75" hidden="1">
       <c r="A137" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="C137" s="4" t="s">
         <v>85</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.75">
+    <row r="138" spans="1:6" ht="15.75" hidden="1">
       <c r="A138" s="1">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="4" t="s">
         <v>85</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.75">
+    <row r="139" spans="1:6" ht="15.75" hidden="1">
       <c r="A139" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>90</v>
+        <v>14</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.75">
+    <row r="140" spans="1:6" ht="15.75" hidden="1">
       <c r="A140" s="1">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>14</v>
@@ -5858,16 +5435,16 @@
         <v>20</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15.75">
+    <row r="141" spans="1:6" ht="15.75" hidden="1">
       <c r="A141" s="1">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>14</v>
@@ -5876,42 +5453,24 @@
         <v>20</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15.75">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E142" s="2"/>
-      <c r="F142" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F142">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F141">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
admin activity and approval
</commit_message>
<xml_diff>
--- a/docs/Admin Task List & Summary.xlsx
+++ b/docs/Admin Task List & Summary.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="100">
   <si>
     <t xml:space="preserve">Sr. NO </t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>Images not submit</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Discount Center Offer</t>
+  </si>
+  <si>
+    <t>Discounts Center List Discounts Center Doctors</t>
   </si>
 </sst>
 </file>
@@ -445,7 +454,467 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="104">
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Eras Medium ITC"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -557,36 +1026,6 @@
         <name val="Eras Medium ITC"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -757,16 +1196,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="shaheryar" refreshedDate="45602.771435069444" createdVersion="8" refreshedVersion="5" minRefreshableVersion="3" recordCount="134">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="shaheryar" refreshedDate="45607.640572569442" createdVersion="8" refreshedVersion="5" minRefreshableVersion="3" recordCount="137">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Sr. NO " numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="140"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="140"/>
     </cacheField>
     <cacheField name="Product" numFmtId="0">
-      <sharedItems count="17">
+      <sharedItems count="18">
         <s v="Clinta Member"/>
         <s v="Dashboard"/>
         <s v="Diseases"/>
@@ -784,10 +1223,11 @@
         <s v="ClinTa Health Care"/>
         <s v="ClinTa Extended"/>
         <s v="ClinTa Pharmacy"/>
+        <s v="Clinta "/>
       </sharedItems>
     </cacheField>
     <cacheField name="Segment" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Sub Segment" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -799,7 +1239,7 @@
       <sharedItems containsBlank="1" count="3">
         <s v="Complete"/>
         <s v="Pending"/>
-        <m u="1"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -812,7 +1252,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="134">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="137">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -1203,7 +1643,7 @@
     <s v="Lab Reports"/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="52"/>
@@ -1211,7 +1651,7 @@
     <s v="Lab Reports"/>
     <s v="Filters"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="53"/>
@@ -1219,7 +1659,7 @@
     <s v="Radiology"/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="54"/>
@@ -1227,7 +1667,7 @@
     <s v="Radiology"/>
     <s v="Filters"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="55"/>
@@ -1299,7 +1739,7 @@
     <s v="Laboratories "/>
     <s v="Filters"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="64"/>
@@ -1339,7 +1779,7 @@
     <s v="Company"/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="73"/>
@@ -1347,7 +1787,7 @@
     <s v="Company"/>
     <s v="Filter"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="74"/>
@@ -1579,7 +2019,7 @@
     <s v="Lab Reports "/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="104"/>
@@ -1587,7 +2027,7 @@
     <s v="Radiology "/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="105"/>
@@ -1595,7 +2035,7 @@
     <s v="Lab Reports "/>
     <s v="Filter"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="106"/>
@@ -1603,7 +2043,7 @@
     <s v="Radiology "/>
     <s v="Filter"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="107"/>
@@ -1611,7 +2051,7 @@
     <s v="Lab Reports Parameters"/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="108"/>
@@ -1619,30 +2059,30 @@
     <s v="Radiology Parameters"/>
     <s v="Crud"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="109"/>
     <x v="13"/>
     <s v="Sponsors"/>
     <s v="Crud"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="110"/>
+    <s v="Image Not Submiit"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
     <x v="13"/>
-    <s v="Sponsors"/>
-    <s v="Filter"/>
-    <m/>
-    <x v="1"/>
+    <s v="Sponsors Product"/>
+    <s v="Crud"/>
+    <s v="Image Not Submiit"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="111"/>
     <x v="13"/>
     <s v="Doctor Websites"/>
     <s v="Crud"/>
-    <m/>
+    <s v="Image Not Submiit"/>
     <x v="1"/>
   </r>
   <r>
@@ -1658,7 +2098,7 @@
     <x v="13"/>
     <s v="Hospital Websites"/>
     <s v="Crud"/>
-    <s v="except Images save"/>
+    <m/>
     <x v="0"/>
   </r>
   <r>
@@ -1667,7 +2107,7 @@
     <s v="Hospital Websites"/>
     <s v="Filter"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="115"/>
@@ -1682,7 +2122,7 @@
     <x v="13"/>
     <s v="General Banners"/>
     <s v="Crud"/>
-    <m/>
+    <s v="Images not submit"/>
     <x v="0"/>
   </r>
   <r>
@@ -1739,7 +2179,7 @@
     <s v="RCCS"/>
     <s v="Filter"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="123"/>
@@ -1750,6 +2190,22 @@
     <x v="1"/>
   </r>
   <r>
+    <m/>
+    <x v="14"/>
+    <s v="Discounts Center List Discounts Center Doctors"/>
+    <s v="Crud"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <x v="14"/>
+    <s v="Discount Center Offer"/>
+    <s v="Crud"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
     <n v="124"/>
     <x v="14"/>
     <s v="Support Vidoes"/>
@@ -1801,8 +2257,8 @@
     <n v="130"/>
     <x v="15"/>
     <s v="Profile"/>
-    <s v="Delete"/>
-    <m/>
+    <s v="Crud"/>
+    <s v="Image Not Submiit"/>
     <x v="1"/>
   </r>
   <r>
@@ -1885,16 +2341,24 @@
     <m/>
     <x v="0"/>
   </r>
+  <r>
+    <m/>
+    <x v="17"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Product Segments" colHeaderCaption=" ">
-  <location ref="A3:D22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Product Segments" colHeaderCaption=" ">
+  <location ref="A3:E23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="18">
+      <items count="19">
         <item x="15"/>
         <item x="14"/>
         <item x="0"/>
@@ -1912,6 +2376,7 @@
         <item x="10"/>
         <item x="12"/>
         <item x="7"/>
+        <item x="17"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1922,7 +2387,7 @@
       <items count="4">
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="2"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1930,7 +2395,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="18">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
@@ -1982,6 +2447,9 @@
     <i>
       <x v="16"/>
     </i>
+    <i>
+      <x v="17"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1989,12 +2457,15 @@
   <colFields count="1">
     <field x="5"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -2004,86 +2475,86 @@
     <dataField name=" " fld="5" subtotal="count" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="27">
-    <format dxfId="37">
+    <format dxfId="103">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="102">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="101">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="100">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="99">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="98">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="92">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="91">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="90">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="89">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="88">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="83">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="82">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2092,7 +2563,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="81">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2101,7 +2572,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="80">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2110,7 +2581,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2119,7 +2590,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="78">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2128,7 +2599,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -2151,11 +2622,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F136" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F138" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="A1:F138">
     <filterColumn colId="1">
       <filters>
-        <filter val="ClinTa Web-Builder"/>
+        <filter val="Main"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2163,12 +2634,12 @@
     <sortCondition ref="A4:A131"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Sr. NO " dataDxfId="5"/>
-    <tableColumn id="1" name="Product" dataDxfId="4"/>
-    <tableColumn id="3" name="Segment" dataDxfId="3"/>
-    <tableColumn id="6" name="Sub Segment" dataDxfId="2"/>
-    <tableColumn id="4" name="Task" dataDxfId="1"/>
-    <tableColumn id="5" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" name="Sr. NO " dataDxfId="74"/>
+    <tableColumn id="1" name="Product" dataDxfId="73"/>
+    <tableColumn id="3" name="Segment" dataDxfId="72"/>
+    <tableColumn id="6" name="Sub Segment" dataDxfId="71"/>
+    <tableColumn id="4" name="Task" dataDxfId="70"/>
+    <tableColumn id="5" name="Status" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2491,11 +2962,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2503,11 +2974,11 @@
     <col min="1" max="1" width="24.375" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="9.125" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.5" customHeight="1">
+    <row r="1" spans="1:5" ht="40.5" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>87</v>
       </c>
@@ -2515,8 +2986,8 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
     </row>
-    <row r="2" spans="1:4" ht="4.5" customHeight="1"/>
-    <row r="3" spans="1:4" ht="18.75" hidden="1">
+    <row r="2" spans="1:5" ht="4.5" customHeight="1"/>
+    <row r="3" spans="1:5" ht="18.75" hidden="1">
       <c r="A3" s="6" t="s">
         <v>86</v>
       </c>
@@ -2525,8 +2996,9 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="18.75">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="6" t="s">
         <v>85</v>
       </c>
@@ -2537,10 +3009,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -2550,25 +3025,27 @@
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9">
-        <v>3</v>
-      </c>
-      <c r="D6" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -2576,11 +3053,12 @@
         <v>4</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -2588,25 +3066,27 @@
         <v>2</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75">
+    <row r="9" spans="1:5" ht="18.75">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75">
+    <row r="10" spans="1:5" ht="18.75">
       <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
@@ -2614,11 +3094,12 @@
       <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75">
+    <row r="11" spans="1:5" ht="18.75">
       <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
@@ -2626,11 +3107,12 @@
         <v>5</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="11">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="14" customFormat="1" ht="18.75">
+    <row r="12" spans="1:5" s="14" customFormat="1" ht="18.75">
       <c r="A12" s="12" t="s">
         <v>42</v>
       </c>
@@ -2638,11 +3120,12 @@
         <v>4</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="13">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75">
       <c r="A13" s="10" t="s">
         <v>43</v>
       </c>
@@ -2650,11 +3133,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="11">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75">
+    <row r="14" spans="1:5" ht="18.75">
       <c r="A14" s="8" t="s">
         <v>49</v>
       </c>
@@ -2664,23 +3148,25 @@
       <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.75">
+    <row r="15" spans="1:5" ht="18.75">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9">
+      <c r="B15" s="9">
         <v>10</v>
       </c>
-      <c r="D15" s="9">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.75">
+    <row r="16" spans="1:5" ht="18.75">
       <c r="A16" s="8" t="s">
         <v>65</v>
       </c>
@@ -2688,11 +3174,12 @@
         <v>8</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="9">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.75">
+    <row r="17" spans="1:5" ht="18.75">
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
@@ -2702,25 +3189,25 @@
       <c r="C17" s="9">
         <v>9</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18.75">
+    <row r="18" spans="1:5" ht="18.75">
       <c r="A18" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="9">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9">
-        <v>2</v>
-      </c>
-      <c r="D18" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.75">
       <c r="A19" s="8" t="s">
         <v>81</v>
       </c>
@@ -2728,11 +3215,12 @@
       <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.75">
+    <row r="20" spans="1:5" ht="18.75">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -2740,36 +3228,46 @@
         <v>4</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="9">
+      <c r="D20" s="9"/>
+      <c r="E20" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18.75">
+    <row r="21" spans="1:5" ht="18.75">
       <c r="A21" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.75">
       <c r="A22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="18.75">
+      <c r="A23" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="9">
-        <v>97</v>
-      </c>
-      <c r="C22" s="9">
-        <v>37</v>
-      </c>
-      <c r="D22" s="9">
-        <v>134</v>
+      <c r="B23" s="9">
+        <v>114</v>
+      </c>
+      <c r="C23" s="9">
+        <v>22</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2782,18 +3280,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomLeft" activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.625" customWidth="1"/>
     <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
@@ -3696,7 +4194,7 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" hidden="1">
@@ -3714,7 +4212,7 @@
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" hidden="1">
@@ -3732,7 +4230,7 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" hidden="1">
@@ -3750,10 +4248,10 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" hidden="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75">
       <c r="A54" s="1">
         <v>55</v>
       </c>
@@ -3771,7 +4269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" hidden="1">
+    <row r="55" spans="1:6" ht="15.75">
       <c r="A55" s="1">
         <v>56</v>
       </c>
@@ -3789,7 +4287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" hidden="1">
+    <row r="56" spans="1:6" ht="15.75">
       <c r="A56" s="1">
         <v>57</v>
       </c>
@@ -3807,7 +4305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" hidden="1">
+    <row r="57" spans="1:6" ht="15.75">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -3825,7 +4323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" hidden="1">
+    <row r="58" spans="1:6" ht="15.75">
       <c r="A58" s="1">
         <v>59</v>
       </c>
@@ -3843,7 +4341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" hidden="1">
+    <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="1">
         <v>60</v>
       </c>
@@ -3861,7 +4359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" hidden="1">
+    <row r="60" spans="1:6" ht="15.75">
       <c r="A60" s="1">
         <v>61</v>
       </c>
@@ -3915,7 +4413,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" hidden="1">
+    <row r="63" spans="1:6" ht="15.75">
       <c r="A63" s="1">
         <v>64</v>
       </c>
@@ -3933,7 +4431,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" hidden="1">
+    <row r="64" spans="1:6" ht="15.75">
       <c r="A64" s="1">
         <v>65</v>
       </c>
@@ -3951,7 +4449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" hidden="1">
+    <row r="65" spans="1:6" ht="15.75">
       <c r="A65" s="1">
         <v>66</v>
       </c>
@@ -3969,7 +4467,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" hidden="1">
+    <row r="66" spans="1:6" ht="15.75">
       <c r="A66" s="1">
         <v>67</v>
       </c>
@@ -4203,7 +4701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" hidden="1">
+    <row r="79" spans="1:6" ht="15.75">
       <c r="A79" s="1">
         <v>84</v>
       </c>
@@ -4542,7 +5040,7 @@
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="15.75" hidden="1">
@@ -4560,7 +5058,7 @@
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="15.75" hidden="1">
@@ -4578,7 +5076,7 @@
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="15.75" hidden="1">
@@ -4596,7 +5094,7 @@
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" hidden="1">
@@ -4614,7 +5112,7 @@
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.75" hidden="1">
@@ -4632,10 +5130,10 @@
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" hidden="1">
       <c r="A103" s="1">
         <v>109</v>
       </c>
@@ -4655,7 +5153,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.75">
+    <row r="104" spans="1:6" ht="15.75" hidden="1">
       <c r="A104" s="2"/>
       <c r="B104" s="1" t="s">
         <v>28</v>
@@ -4673,7 +5171,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.75">
+    <row r="105" spans="1:6" ht="15.75" hidden="1">
       <c r="A105" s="1">
         <v>111</v>
       </c>
@@ -4693,7 +5191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.75">
+    <row r="106" spans="1:6" ht="15.75" hidden="1">
       <c r="A106" s="1">
         <v>112</v>
       </c>
@@ -4711,7 +5209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.75">
+    <row r="107" spans="1:6" ht="15.75" hidden="1">
       <c r="A107" s="1">
         <v>113</v>
       </c>
@@ -4729,7 +5227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.75">
+    <row r="108" spans="1:6" ht="15.75" hidden="1">
       <c r="A108" s="1">
         <v>114</v>
       </c>
@@ -4747,7 +5245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.75">
+    <row r="109" spans="1:6" ht="15.75" hidden="1">
       <c r="A109" s="1">
         <v>115</v>
       </c>
@@ -4765,7 +5263,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.75">
+    <row r="110" spans="1:6" ht="15.75" hidden="1">
       <c r="A110" s="1">
         <v>116</v>
       </c>
@@ -4930,44 +5428,40 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="15.75" hidden="1">
-      <c r="A119" s="1">
-        <v>124</v>
-      </c>
+      <c r="A119" s="2"/>
       <c r="B119" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E119" s="2"/>
       <c r="F119" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1">
-      <c r="A120" s="1">
-        <v>125</v>
-      </c>
+      <c r="A120" s="2"/>
       <c r="B120" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>25</v>
+        <v>98</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1">
       <c r="A121" s="1">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>14</v>
@@ -4975,17 +5469,17 @@
       <c r="C121" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E121" s="2"/>
+      <c r="D121" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15.75" hidden="1">
       <c r="A122" s="1">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>14</v>
@@ -4994,7 +5488,7 @@
         <v>19</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="1" t="s">
@@ -5003,108 +5497,108 @@
     </row>
     <row r="123" spans="1:6" ht="15.75" hidden="1">
       <c r="A123" s="1">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E123" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123" s="2"/>
       <c r="F123" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15.75" hidden="1">
       <c r="A124" s="1">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E124" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="E124" s="2"/>
       <c r="F124" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15.75" hidden="1">
       <c r="A125" s="1">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15.75" hidden="1">
       <c r="A126" s="1">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="15.75" hidden="1">
       <c r="A127" s="1">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="1"/>
+      <c r="E127" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F127" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="15.75" hidden="1">
       <c r="A128" s="1">
-        <v>133</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>26</v>
+        <v>131</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
@@ -5113,16 +5607,16 @@
     </row>
     <row r="129" spans="1:6" ht="15.75" hidden="1">
       <c r="A129" s="1">
-        <v>134</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>26</v>
+        <v>132</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
@@ -5131,43 +5625,43 @@
     </row>
     <row r="130" spans="1:6" ht="15.75" hidden="1">
       <c r="A130" s="1">
-        <v>135</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E130" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="15.75" hidden="1">
       <c r="A131" s="1">
-        <v>136</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E131" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="15.75" hidden="1">
       <c r="A132" s="1">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>82</v>
@@ -5176,7 +5670,7 @@
         <v>83</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="1" t="s">
@@ -5185,16 +5679,16 @@
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1">
       <c r="A133" s="1">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>25</v>
+        <v>82</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="1" t="s">
@@ -5203,16 +5697,16 @@
     </row>
     <row r="134" spans="1:6" ht="15.75" hidden="1">
       <c r="A134" s="1">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>24</v>
+        <v>82</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="1" t="s">
@@ -5221,7 +5715,7 @@
     </row>
     <row r="135" spans="1:6" ht="15.75" hidden="1">
       <c r="A135" s="1">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>14</v>
@@ -5230,7 +5724,7 @@
         <v>20</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="1" t="s">
@@ -5238,26 +5732,62 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1">
-      <c r="A136" s="2"/>
+      <c r="A136" s="1">
+        <v>139</v>
+      </c>
       <c r="B136" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15.75" hidden="1">
+      <c r="A137" s="1">
+        <v>140</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="15.75" hidden="1">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F136">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F138">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>